<commit_message>
Update: fixes for use with Ruby 2.0.0
</commit_message>
<xml_diff>
--- a/public/test/template_test.xlsx
+++ b/public/test/template_test.xlsx
@@ -28,7 +28,7 @@
     <t>title</t>
   </si>
   <si>
-    <t>Title-nonsort</t>
+    <t>title-nonsort</t>
   </si>
   <si>
     <t>title-alternative</t>
@@ -236,10 +236,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="@" numFmtId="165"/>
-    <numFmt formatCode="@" numFmtId="166"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -340,7 +339,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -373,15 +372,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -464,8 +459,8 @@
   </sheetPr>
   <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D5" activeCellId="0" pane="topLeft" sqref="D5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="AF1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="AG8" activeCellId="0" pane="topLeft" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -475,7 +470,7 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.9959514170041"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="23"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.1417004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="36.1417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.4089068825911"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.2793522267206"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.7165991902834"/>
@@ -552,7 +547,7 @@
       <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="5" t="s">
@@ -570,7 +565,7 @@
       <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="V1" s="4" t="s">
@@ -603,13 +598,13 @@
       <c r="AE1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AF1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AH1" s="8" t="s">
         <v>30</v>
       </c>
       <c r="AI1" s="4" t="s">
@@ -624,70 +619,70 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="T2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="V2" s="9" t="s">
         <v>55</v>
       </c>
       <c r="W2" s="1" t="s">

</xml_diff>